<commit_message>
Ajout de plusieurs articles dont le dernier en date de Daniel
</commit_message>
<xml_diff>
--- a/Bibliographie.xlsx
+++ b/Bibliographie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yberton\Documents\Bibliographie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDB308F-F609-43BA-BB14-7BA32DF4C867}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E4214A-1096-4D3D-A460-56BCA798FB02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{08986EE9-D4D5-48AB-A032-B91F14669D29}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{08986EE9-D4D5-48AB-A032-B91F14669D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>dP/dz</t>
   </si>
@@ -199,10 +199,6 @@
     <t>R744</t>
   </si>
   <si>
-    <t>q"
-[w/m²/s]</t>
-  </si>
-  <si>
     <t>ONB</t>
   </si>
   <si>
@@ -231,6 +227,20 @@
   </si>
   <si>
     <t>[60 ; 120]</t>
+  </si>
+  <si>
+    <t>Flow boiling of R245fa in 1.1 mm diameter stainless steel, 
+brass and copper tubes</t>
+  </si>
+  <si>
+    <t>[E.A. Pike-Wilson, T.G. Karayiannis]</t>
+  </si>
+  <si>
+    <t>q"
+[kW/m²]</t>
+  </si>
+  <si>
+    <t>[10 ; 60]</t>
   </si>
 </sst>
 </file>
@@ -714,41 +724,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39E5EE1-A7F3-4A60-8E56-91CF6268836E}">
   <dimension ref="A1:AB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="57" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="64.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="10" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5" style="1" customWidth="1"/>
+    <col min="15" max="16" width="7.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10" style="1" customWidth="1"/>
-    <col min="25" max="25" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>23</v>
@@ -766,7 +777,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>19</v>
@@ -790,13 +801,13 @@
         <v>43</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>0</v>
@@ -817,13 +828,13 @@
         <v>15</v>
       </c>
       <c r="X1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>24</v>
@@ -889,7 +900,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
       <c r="AB2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
@@ -1134,7 +1145,7 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -1175,23 +1186,35 @@
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+    <row r="8" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2014</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
+      <c r="Q8" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -1652,12 +1675,12 @@
       <c r="AA24" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:L2 K4:L4 C3:F3 H3:L3 H4:I4 B1:L1 B2:F2 H2:I2 B7:L46 B4:F6 H5:L6 M1:AL46">
+  <conditionalFormatting sqref="K2:L2 K4:L4 C3:F3 H3:L3 H4:I4 B1:L1 B2:F2 H2:I2 B4:F6 H5:L6 M1:AL46 B7:L46">
     <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:L2 K4:L4 C3:F3 H3:L3 H4:I4 B2:F2 H2:I2 B7:L46 B4:F6 H5:L6 M2:AL46">
+  <conditionalFormatting sqref="K2:L2 K4:L4 C3:F3 H3:L3 H4:I4 B2:F2 H2:I2 B4:F6 H5:L6 M2:AL46 B7:L46">
     <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"V"</formula>
     </cfRule>

</xml_diff>